<commit_message>
feature: Revising graphs for paper.
</commit_message>
<xml_diff>
--- a/data/processed/ERC20_most_rec_token_type.xlsx
+++ b/data/processed/ERC20_most_rec_token_type.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="281">
+  <si>
+    <t>count</t>
+  </si>
   <si>
     <t>ERC20_most_rec_token_type</t>
   </si>
@@ -1218,13 +1221,16 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>40.15604681404421</v>
@@ -1232,7 +1238,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>20.26007802340702</v>
@@ -1240,7 +1246,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>9.232769830949286</v>
@@ -1248,7 +1254,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>2.106631989596879</v>
@@ -1256,7 +1262,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>2.080624187256177</v>
@@ -1264,7 +1270,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>1.404421326397919</v>
@@ -1272,7 +1278,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>1.378413524057217</v>
@@ -1280,7 +1286,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>1.222366710013004</v>
@@ -1288,7 +1294,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>1.1703511053316</v>
@@ -1296,7 +1302,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>0.9622886866059818</v>
@@ -1304,7 +1310,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>0.9622886866059818</v>
@@ -1312,7 +1318,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <v>0.9102730819245773</v>
@@ -1320,7 +1326,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14">
         <v>0.8582574772431729</v>
@@ -1328,7 +1334,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15">
         <v>0.7542262678803641</v>
@@ -1336,7 +1342,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16">
         <v>0.6762028608582574</v>
@@ -1344,7 +1350,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17">
         <v>0.6241872561768531</v>
@@ -1352,7 +1358,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <v>0.5201560468140443</v>
@@ -1360,7 +1366,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19">
         <v>0.494148244473342</v>
@@ -1368,7 +1374,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20">
         <v>0.494148244473342</v>
@@ -1376,7 +1382,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21">
         <v>0.4681404421326398</v>
@@ -1384,7 +1390,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22">
         <v>0.3381014304291287</v>
@@ -1392,7 +1398,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23">
         <v>0.3120936280884266</v>
@@ -1400,7 +1406,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24">
         <v>0.3120936280884266</v>
@@ -1408,7 +1414,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25">
         <v>0.2340702210663199</v>
@@ -1416,7 +1422,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26">
         <v>0.2340702210663199</v>
@@ -1424,7 +1430,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27">
         <v>0.2340702210663199</v>
@@ -1432,7 +1438,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28">
         <v>0.2080624187256177</v>
@@ -1440,7 +1446,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29">
         <v>0.2080624187256177</v>
@@ -1448,7 +1454,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B30">
         <v>0.2080624187256177</v>
@@ -1456,7 +1462,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B31">
         <v>0.2080624187256177</v>
@@ -1464,7 +1470,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B32">
         <v>0.1820546163849155</v>
@@ -1472,7 +1478,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B33">
         <v>0.1820546163849155</v>
@@ -1480,7 +1486,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B34">
         <v>0.1560468140442133</v>
@@ -1488,7 +1494,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B35">
         <v>0.1560468140442133</v>
@@ -1496,7 +1502,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B36">
         <v>0.1560468140442133</v>
@@ -1504,7 +1510,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B37">
         <v>0.1560468140442133</v>
@@ -1512,7 +1518,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B38">
         <v>0.1300390117035111</v>
@@ -1520,7 +1526,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B39">
         <v>0.1300390117035111</v>
@@ -1528,7 +1534,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B40">
         <v>0.1300390117035111</v>
@@ -1536,7 +1542,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B41">
         <v>0.1300390117035111</v>
@@ -1544,7 +1550,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B42">
         <v>0.1040312093628088</v>
@@ -1552,7 +1558,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B43">
         <v>0.1040312093628088</v>
@@ -1560,7 +1566,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B44">
         <v>0.1040312093628088</v>
@@ -1568,7 +1574,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B45">
         <v>0.1040312093628088</v>
@@ -1576,7 +1582,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B46">
         <v>0.1040312093628088</v>
@@ -1584,7 +1590,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B47">
         <v>0.1040312093628088</v>
@@ -1592,7 +1598,7 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B48">
         <v>0.1040312093628088</v>
@@ -1600,7 +1606,7 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B49">
         <v>0.1040312093628088</v>
@@ -1608,7 +1614,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B50">
         <v>0.1040312093628088</v>
@@ -1616,7 +1622,7 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B51">
         <v>0.1040312093628088</v>
@@ -1624,7 +1630,7 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B52">
         <v>0.07802340702210664</v>
@@ -1632,7 +1638,7 @@
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B53">
         <v>0.07802340702210664</v>
@@ -1640,7 +1646,7 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B54">
         <v>0.07802340702210664</v>
@@ -1648,7 +1654,7 @@
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B55">
         <v>0.07802340702210664</v>
@@ -1656,7 +1662,7 @@
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B56">
         <v>0.07802340702210664</v>
@@ -1664,7 +1670,7 @@
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B57">
         <v>0.07802340702210664</v>
@@ -1672,7 +1678,7 @@
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B58">
         <v>0.07802340702210664</v>
@@ -1680,7 +1686,7 @@
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B59">
         <v>0.07802340702210664</v>
@@ -1688,7 +1694,7 @@
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B60">
         <v>0.07802340702210664</v>
@@ -1696,7 +1702,7 @@
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B61">
         <v>0.07802340702210664</v>
@@ -1704,7 +1710,7 @@
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B62">
         <v>0.07802340702210664</v>
@@ -1712,7 +1718,7 @@
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B63">
         <v>0.07802340702210664</v>
@@ -1720,7 +1726,7 @@
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B64">
         <v>0.07802340702210664</v>
@@ -1728,7 +1734,7 @@
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B65">
         <v>0.07802340702210664</v>
@@ -1736,7 +1742,7 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B66">
         <v>0.07802340702210664</v>
@@ -1744,7 +1750,7 @@
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B67">
         <v>0.07802340702210664</v>
@@ -1752,7 +1758,7 @@
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B68">
         <v>0.07802340702210664</v>
@@ -1760,7 +1766,7 @@
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B69">
         <v>0.07802340702210664</v>
@@ -1768,7 +1774,7 @@
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B70">
         <v>0.07802340702210664</v>
@@ -1776,7 +1782,7 @@
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B71">
         <v>0.05201560468140442</v>
@@ -1784,7 +1790,7 @@
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B72">
         <v>0.05201560468140442</v>
@@ -1792,7 +1798,7 @@
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B73">
         <v>0.05201560468140442</v>
@@ -1800,7 +1806,7 @@
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B74">
         <v>0.05201560468140442</v>
@@ -1808,7 +1814,7 @@
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B75">
         <v>0.05201560468140442</v>
@@ -1816,7 +1822,7 @@
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B76">
         <v>0.05201560468140442</v>
@@ -1824,7 +1830,7 @@
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B77">
         <v>0.05201560468140442</v>
@@ -1832,7 +1838,7 @@
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B78">
         <v>0.05201560468140442</v>
@@ -1840,7 +1846,7 @@
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B79">
         <v>0.05201560468140442</v>
@@ -1848,7 +1854,7 @@
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B80">
         <v>0.05201560468140442</v>
@@ -1856,7 +1862,7 @@
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B81">
         <v>0.05201560468140442</v>
@@ -1864,7 +1870,7 @@
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B82">
         <v>0.05201560468140442</v>
@@ -1872,7 +1878,7 @@
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B83">
         <v>0.05201560468140442</v>
@@ -1880,7 +1886,7 @@
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B84">
         <v>0.05201560468140442</v>
@@ -1888,7 +1894,7 @@
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B85">
         <v>0.05201560468140442</v>
@@ -1896,7 +1902,7 @@
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B86">
         <v>0.05201560468140442</v>
@@ -1904,7 +1910,7 @@
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B87">
         <v>0.05201560468140442</v>
@@ -1912,7 +1918,7 @@
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B88">
         <v>0.05201560468140442</v>
@@ -1920,7 +1926,7 @@
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B89">
         <v>0.05201560468140442</v>
@@ -1928,7 +1934,7 @@
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B90">
         <v>0.05201560468140442</v>
@@ -1936,7 +1942,7 @@
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B91">
         <v>0.05201560468140442</v>
@@ -1944,7 +1950,7 @@
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B92">
         <v>0.05201560468140442</v>
@@ -1952,7 +1958,7 @@
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B93">
         <v>0.05201560468140442</v>
@@ -1960,7 +1966,7 @@
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B94">
         <v>0.05201560468140442</v>
@@ -1968,7 +1974,7 @@
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B95">
         <v>0.05201560468140442</v>
@@ -1976,7 +1982,7 @@
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B96">
         <v>0.05201560468140442</v>
@@ -1984,7 +1990,7 @@
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B97">
         <v>0.05201560468140442</v>
@@ -1992,7 +1998,7 @@
     </row>
     <row r="98" spans="1:2">
       <c r="A98" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B98">
         <v>0.05201560468140442</v>
@@ -2000,7 +2006,7 @@
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B99">
         <v>0.05201560468140442</v>
@@ -2008,7 +2014,7 @@
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B100">
         <v>0.05201560468140442</v>
@@ -2016,7 +2022,7 @@
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B101">
         <v>0.05201560468140442</v>
@@ -2024,7 +2030,7 @@
     </row>
     <row r="102" spans="1:2">
       <c r="A102" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B102">
         <v>0.05201560468140442</v>
@@ -2032,7 +2038,7 @@
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B103">
         <v>0.05201560468140442</v>
@@ -2040,7 +2046,7 @@
     </row>
     <row r="104" spans="1:2">
       <c r="A104" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B104">
         <v>0.05201560468140442</v>
@@ -2048,7 +2054,7 @@
     </row>
     <row r="105" spans="1:2">
       <c r="A105" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B105">
         <v>0.05201560468140442</v>
@@ -2056,7 +2062,7 @@
     </row>
     <row r="106" spans="1:2">
       <c r="A106" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B106">
         <v>0.05201560468140442</v>
@@ -2064,7 +2070,7 @@
     </row>
     <row r="107" spans="1:2">
       <c r="A107" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B107">
         <v>0.05201560468140442</v>
@@ -2072,7 +2078,7 @@
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B108">
         <v>0.05201560468140442</v>
@@ -2080,7 +2086,7 @@
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B109">
         <v>0.05201560468140442</v>
@@ -2088,7 +2094,7 @@
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B110">
         <v>0.05201560468140442</v>
@@ -2096,7 +2102,7 @@
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B111">
         <v>0.05201560468140442</v>
@@ -2104,7 +2110,7 @@
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B112">
         <v>0.05201560468140442</v>
@@ -2112,7 +2118,7 @@
     </row>
     <row r="113" spans="1:2">
       <c r="A113" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B113">
         <v>0.05201560468140442</v>
@@ -2120,7 +2126,7 @@
     </row>
     <row r="114" spans="1:2">
       <c r="A114" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B114">
         <v>0.05201560468140442</v>
@@ -2128,7 +2134,7 @@
     </row>
     <row r="115" spans="1:2">
       <c r="A115" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B115">
         <v>0.05201560468140442</v>
@@ -2136,7 +2142,7 @@
     </row>
     <row r="116" spans="1:2">
       <c r="A116" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B116">
         <v>0.05201560468140442</v>
@@ -2144,7 +2150,7 @@
     </row>
     <row r="117" spans="1:2">
       <c r="A117" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B117">
         <v>0.05201560468140442</v>
@@ -2152,7 +2158,7 @@
     </row>
     <row r="118" spans="1:2">
       <c r="A118" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B118">
         <v>0.05201560468140442</v>
@@ -2160,7 +2166,7 @@
     </row>
     <row r="119" spans="1:2">
       <c r="A119" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B119">
         <v>0.05201560468140442</v>
@@ -2168,7 +2174,7 @@
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B120">
         <v>0.02600780234070221</v>
@@ -2176,7 +2182,7 @@
     </row>
     <row r="121" spans="1:2">
       <c r="A121" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B121">
         <v>0.02600780234070221</v>
@@ -2184,7 +2190,7 @@
     </row>
     <row r="122" spans="1:2">
       <c r="A122" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B122">
         <v>0.02600780234070221</v>
@@ -2192,7 +2198,7 @@
     </row>
     <row r="123" spans="1:2">
       <c r="A123" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B123">
         <v>0.02600780234070221</v>
@@ -2200,7 +2206,7 @@
     </row>
     <row r="124" spans="1:2">
       <c r="A124" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B124">
         <v>0.02600780234070221</v>
@@ -2208,7 +2214,7 @@
     </row>
     <row r="125" spans="1:2">
       <c r="A125" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B125">
         <v>0.02600780234070221</v>
@@ -2216,7 +2222,7 @@
     </row>
     <row r="126" spans="1:2">
       <c r="A126" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B126">
         <v>0.02600780234070221</v>
@@ -2224,7 +2230,7 @@
     </row>
     <row r="127" spans="1:2">
       <c r="A127" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B127">
         <v>0.02600780234070221</v>
@@ -2232,7 +2238,7 @@
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B128">
         <v>0.02600780234070221</v>
@@ -2240,7 +2246,7 @@
     </row>
     <row r="129" spans="1:2">
       <c r="A129" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B129">
         <v>0.02600780234070221</v>
@@ -2248,7 +2254,7 @@
     </row>
     <row r="130" spans="1:2">
       <c r="A130" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B130">
         <v>0.02600780234070221</v>
@@ -2256,7 +2262,7 @@
     </row>
     <row r="131" spans="1:2">
       <c r="A131" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B131">
         <v>0.02600780234070221</v>
@@ -2264,7 +2270,7 @@
     </row>
     <row r="132" spans="1:2">
       <c r="A132" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B132">
         <v>0.02600780234070221</v>
@@ -2272,7 +2278,7 @@
     </row>
     <row r="133" spans="1:2">
       <c r="A133" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B133">
         <v>0.02600780234070221</v>
@@ -2280,7 +2286,7 @@
     </row>
     <row r="134" spans="1:2">
       <c r="A134" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B134">
         <v>0.02600780234070221</v>
@@ -2288,7 +2294,7 @@
     </row>
     <row r="135" spans="1:2">
       <c r="A135" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B135">
         <v>0.02600780234070221</v>
@@ -2296,7 +2302,7 @@
     </row>
     <row r="136" spans="1:2">
       <c r="A136" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B136">
         <v>0.02600780234070221</v>
@@ -2304,7 +2310,7 @@
     </row>
     <row r="137" spans="1:2">
       <c r="A137" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B137">
         <v>0.02600780234070221</v>
@@ -2312,7 +2318,7 @@
     </row>
     <row r="138" spans="1:2">
       <c r="A138" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B138">
         <v>0.02600780234070221</v>
@@ -2320,7 +2326,7 @@
     </row>
     <row r="139" spans="1:2">
       <c r="A139" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B139">
         <v>0.02600780234070221</v>
@@ -2328,7 +2334,7 @@
     </row>
     <row r="140" spans="1:2">
       <c r="A140" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B140">
         <v>0.02600780234070221</v>
@@ -2336,7 +2342,7 @@
     </row>
     <row r="141" spans="1:2">
       <c r="A141" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B141">
         <v>0.02600780234070221</v>
@@ -2344,7 +2350,7 @@
     </row>
     <row r="142" spans="1:2">
       <c r="A142" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B142">
         <v>0.02600780234070221</v>
@@ -2352,7 +2358,7 @@
     </row>
     <row r="143" spans="1:2">
       <c r="A143" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B143">
         <v>0.02600780234070221</v>
@@ -2360,7 +2366,7 @@
     </row>
     <row r="144" spans="1:2">
       <c r="A144" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B144">
         <v>0.02600780234070221</v>
@@ -2368,7 +2374,7 @@
     </row>
     <row r="145" spans="1:2">
       <c r="A145" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B145">
         <v>0.02600780234070221</v>
@@ -2376,7 +2382,7 @@
     </row>
     <row r="146" spans="1:2">
       <c r="A146" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B146">
         <v>0.02600780234070221</v>
@@ -2384,7 +2390,7 @@
     </row>
     <row r="147" spans="1:2">
       <c r="A147" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B147">
         <v>0.02600780234070221</v>
@@ -2392,7 +2398,7 @@
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B148">
         <v>0.02600780234070221</v>
@@ -2400,7 +2406,7 @@
     </row>
     <row r="149" spans="1:2">
       <c r="A149" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B149">
         <v>0.02600780234070221</v>
@@ -2408,7 +2414,7 @@
     </row>
     <row r="150" spans="1:2">
       <c r="A150" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B150">
         <v>0.02600780234070221</v>
@@ -2416,7 +2422,7 @@
     </row>
     <row r="151" spans="1:2">
       <c r="A151" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B151">
         <v>0.02600780234070221</v>
@@ -2424,7 +2430,7 @@
     </row>
     <row r="152" spans="1:2">
       <c r="A152" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B152">
         <v>0.02600780234070221</v>
@@ -2432,7 +2438,7 @@
     </row>
     <row r="153" spans="1:2">
       <c r="A153" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B153">
         <v>0.02600780234070221</v>
@@ -2440,7 +2446,7 @@
     </row>
     <row r="154" spans="1:2">
       <c r="A154" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B154">
         <v>0.02600780234070221</v>
@@ -2448,7 +2454,7 @@
     </row>
     <row r="155" spans="1:2">
       <c r="A155" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B155">
         <v>0.02600780234070221</v>
@@ -2456,7 +2462,7 @@
     </row>
     <row r="156" spans="1:2">
       <c r="A156" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B156">
         <v>0.02600780234070221</v>
@@ -2464,7 +2470,7 @@
     </row>
     <row r="157" spans="1:2">
       <c r="A157" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B157">
         <v>0.02600780234070221</v>
@@ -2472,7 +2478,7 @@
     </row>
     <row r="158" spans="1:2">
       <c r="A158" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B158">
         <v>0.02600780234070221</v>
@@ -2480,7 +2486,7 @@
     </row>
     <row r="159" spans="1:2">
       <c r="A159" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B159">
         <v>0.02600780234070221</v>
@@ -2488,7 +2494,7 @@
     </row>
     <row r="160" spans="1:2">
       <c r="A160" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B160">
         <v>0.02600780234070221</v>
@@ -2496,7 +2502,7 @@
     </row>
     <row r="161" spans="1:2">
       <c r="A161" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B161">
         <v>0.02600780234070221</v>
@@ -2504,7 +2510,7 @@
     </row>
     <row r="162" spans="1:2">
       <c r="A162" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B162">
         <v>0.02600780234070221</v>
@@ -2512,7 +2518,7 @@
     </row>
     <row r="163" spans="1:2">
       <c r="A163" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B163">
         <v>0.02600780234070221</v>
@@ -2520,7 +2526,7 @@
     </row>
     <row r="164" spans="1:2">
       <c r="A164" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B164">
         <v>0.02600780234070221</v>
@@ -2528,7 +2534,7 @@
     </row>
     <row r="165" spans="1:2">
       <c r="A165" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B165">
         <v>0.02600780234070221</v>
@@ -2536,7 +2542,7 @@
     </row>
     <row r="166" spans="1:2">
       <c r="A166" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B166">
         <v>0.02600780234070221</v>
@@ -2544,7 +2550,7 @@
     </row>
     <row r="167" spans="1:2">
       <c r="A167" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B167">
         <v>0.02600780234070221</v>
@@ -2552,7 +2558,7 @@
     </row>
     <row r="168" spans="1:2">
       <c r="A168" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B168">
         <v>0.02600780234070221</v>
@@ -2560,7 +2566,7 @@
     </row>
     <row r="169" spans="1:2">
       <c r="A169" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B169">
         <v>0.02600780234070221</v>
@@ -2568,7 +2574,7 @@
     </row>
     <row r="170" spans="1:2">
       <c r="A170" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B170">
         <v>0.02600780234070221</v>
@@ -2576,7 +2582,7 @@
     </row>
     <row r="171" spans="1:2">
       <c r="A171" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B171">
         <v>0.02600780234070221</v>
@@ -2584,7 +2590,7 @@
     </row>
     <row r="172" spans="1:2">
       <c r="A172" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B172">
         <v>0.02600780234070221</v>
@@ -2592,7 +2598,7 @@
     </row>
     <row r="173" spans="1:2">
       <c r="A173" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B173">
         <v>0.02600780234070221</v>
@@ -2600,7 +2606,7 @@
     </row>
     <row r="174" spans="1:2">
       <c r="A174" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B174">
         <v>0.02600780234070221</v>
@@ -2608,7 +2614,7 @@
     </row>
     <row r="175" spans="1:2">
       <c r="A175" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B175">
         <v>0.02600780234070221</v>
@@ -2616,7 +2622,7 @@
     </row>
     <row r="176" spans="1:2">
       <c r="A176" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B176">
         <v>0.02600780234070221</v>
@@ -2624,7 +2630,7 @@
     </row>
     <row r="177" spans="1:2">
       <c r="A177" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B177">
         <v>0.02600780234070221</v>
@@ -2632,7 +2638,7 @@
     </row>
     <row r="178" spans="1:2">
       <c r="A178" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B178">
         <v>0.02600780234070221</v>
@@ -2640,7 +2646,7 @@
     </row>
     <row r="179" spans="1:2">
       <c r="A179" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B179">
         <v>0.02600780234070221</v>
@@ -2648,7 +2654,7 @@
     </row>
     <row r="180" spans="1:2">
       <c r="A180" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B180">
         <v>0.02600780234070221</v>
@@ -2656,7 +2662,7 @@
     </row>
     <row r="181" spans="1:2">
       <c r="A181" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B181">
         <v>0.02600780234070221</v>
@@ -2664,7 +2670,7 @@
     </row>
     <row r="182" spans="1:2">
       <c r="A182" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B182">
         <v>0.02600780234070221</v>
@@ -2672,7 +2678,7 @@
     </row>
     <row r="183" spans="1:2">
       <c r="A183" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B183">
         <v>0.02600780234070221</v>
@@ -2680,7 +2686,7 @@
     </row>
     <row r="184" spans="1:2">
       <c r="A184" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B184">
         <v>0.02600780234070221</v>
@@ -2688,7 +2694,7 @@
     </row>
     <row r="185" spans="1:2">
       <c r="A185" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B185">
         <v>0.02600780234070221</v>
@@ -2696,7 +2702,7 @@
     </row>
     <row r="186" spans="1:2">
       <c r="A186" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B186">
         <v>0.02600780234070221</v>
@@ -2704,7 +2710,7 @@
     </row>
     <row r="187" spans="1:2">
       <c r="A187" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B187">
         <v>0.02600780234070221</v>
@@ -2712,7 +2718,7 @@
     </row>
     <row r="188" spans="1:2">
       <c r="A188" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B188">
         <v>0.02600780234070221</v>
@@ -2720,7 +2726,7 @@
     </row>
     <row r="189" spans="1:2">
       <c r="A189" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B189">
         <v>0.02600780234070221</v>
@@ -2728,7 +2734,7 @@
     </row>
     <row r="190" spans="1:2">
       <c r="A190" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B190">
         <v>0.02600780234070221</v>
@@ -2736,7 +2742,7 @@
     </row>
     <row r="191" spans="1:2">
       <c r="A191" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B191">
         <v>0.02600780234070221</v>
@@ -2744,7 +2750,7 @@
     </row>
     <row r="192" spans="1:2">
       <c r="A192" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B192">
         <v>0.02600780234070221</v>
@@ -2752,7 +2758,7 @@
     </row>
     <row r="193" spans="1:2">
       <c r="A193" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B193">
         <v>0.02600780234070221</v>
@@ -2760,7 +2766,7 @@
     </row>
     <row r="194" spans="1:2">
       <c r="A194" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B194">
         <v>0.02600780234070221</v>
@@ -2768,7 +2774,7 @@
     </row>
     <row r="195" spans="1:2">
       <c r="A195" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B195">
         <v>0.02600780234070221</v>
@@ -2776,7 +2782,7 @@
     </row>
     <row r="196" spans="1:2">
       <c r="A196" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B196">
         <v>0.02600780234070221</v>
@@ -2784,7 +2790,7 @@
     </row>
     <row r="197" spans="1:2">
       <c r="A197" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B197">
         <v>0.02600780234070221</v>
@@ -2792,7 +2798,7 @@
     </row>
     <row r="198" spans="1:2">
       <c r="A198" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B198">
         <v>0.02600780234070221</v>
@@ -2800,7 +2806,7 @@
     </row>
     <row r="199" spans="1:2">
       <c r="A199" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B199">
         <v>0.02600780234070221</v>
@@ -2808,7 +2814,7 @@
     </row>
     <row r="200" spans="1:2">
       <c r="A200" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B200">
         <v>0.02600780234070221</v>
@@ -2816,7 +2822,7 @@
     </row>
     <row r="201" spans="1:2">
       <c r="A201" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B201">
         <v>0.02600780234070221</v>
@@ -2824,7 +2830,7 @@
     </row>
     <row r="202" spans="1:2">
       <c r="A202" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B202">
         <v>0.02600780234070221</v>
@@ -2832,7 +2838,7 @@
     </row>
     <row r="203" spans="1:2">
       <c r="A203" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B203">
         <v>0.02600780234070221</v>
@@ -2840,7 +2846,7 @@
     </row>
     <row r="204" spans="1:2">
       <c r="A204" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B204">
         <v>0.02600780234070221</v>
@@ -2848,7 +2854,7 @@
     </row>
     <row r="205" spans="1:2">
       <c r="A205" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B205">
         <v>0.02600780234070221</v>
@@ -2856,7 +2862,7 @@
     </row>
     <row r="206" spans="1:2">
       <c r="A206" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B206">
         <v>0.02600780234070221</v>
@@ -2864,7 +2870,7 @@
     </row>
     <row r="207" spans="1:2">
       <c r="A207" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B207">
         <v>0.02600780234070221</v>
@@ -2872,7 +2878,7 @@
     </row>
     <row r="208" spans="1:2">
       <c r="A208" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B208">
         <v>0.02600780234070221</v>
@@ -2880,7 +2886,7 @@
     </row>
     <row r="209" spans="1:2">
       <c r="A209" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B209">
         <v>0.02600780234070221</v>
@@ -2888,7 +2894,7 @@
     </row>
     <row r="210" spans="1:2">
       <c r="A210" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B210">
         <v>0.02600780234070221</v>
@@ -2896,7 +2902,7 @@
     </row>
     <row r="211" spans="1:2">
       <c r="A211" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B211">
         <v>0.02600780234070221</v>
@@ -2904,7 +2910,7 @@
     </row>
     <row r="212" spans="1:2">
       <c r="A212" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B212">
         <v>0.02600780234070221</v>
@@ -2912,7 +2918,7 @@
     </row>
     <row r="213" spans="1:2">
       <c r="A213" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B213">
         <v>0.02600780234070221</v>
@@ -2920,7 +2926,7 @@
     </row>
     <row r="214" spans="1:2">
       <c r="A214" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B214">
         <v>0.02600780234070221</v>
@@ -2928,7 +2934,7 @@
     </row>
     <row r="215" spans="1:2">
       <c r="A215" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B215">
         <v>0.02600780234070221</v>
@@ -2936,7 +2942,7 @@
     </row>
     <row r="216" spans="1:2">
       <c r="A216" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B216">
         <v>0.02600780234070221</v>
@@ -2944,7 +2950,7 @@
     </row>
     <row r="217" spans="1:2">
       <c r="A217" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B217">
         <v>0.02600780234070221</v>
@@ -2952,7 +2958,7 @@
     </row>
     <row r="218" spans="1:2">
       <c r="A218" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B218">
         <v>0.02600780234070221</v>
@@ -2960,7 +2966,7 @@
     </row>
     <row r="219" spans="1:2">
       <c r="A219" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B219">
         <v>0.02600780234070221</v>
@@ -2968,7 +2974,7 @@
     </row>
     <row r="220" spans="1:2">
       <c r="A220" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B220">
         <v>0.02600780234070221</v>
@@ -2976,7 +2982,7 @@
     </row>
     <row r="221" spans="1:2">
       <c r="A221" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B221">
         <v>0.02600780234070221</v>
@@ -2984,7 +2990,7 @@
     </row>
     <row r="222" spans="1:2">
       <c r="A222" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B222">
         <v>0.02600780234070221</v>
@@ -2992,7 +2998,7 @@
     </row>
     <row r="223" spans="1:2">
       <c r="A223" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B223">
         <v>0.02600780234070221</v>
@@ -3000,7 +3006,7 @@
     </row>
     <row r="224" spans="1:2">
       <c r="A224" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B224">
         <v>0.02600780234070221</v>
@@ -3008,7 +3014,7 @@
     </row>
     <row r="225" spans="1:2">
       <c r="A225" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B225">
         <v>0.02600780234070221</v>
@@ -3016,7 +3022,7 @@
     </row>
     <row r="226" spans="1:2">
       <c r="A226" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B226">
         <v>0.02600780234070221</v>
@@ -3024,7 +3030,7 @@
     </row>
     <row r="227" spans="1:2">
       <c r="A227" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B227">
         <v>0.02600780234070221</v>
@@ -3032,7 +3038,7 @@
     </row>
     <row r="228" spans="1:2">
       <c r="A228" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B228">
         <v>0.02600780234070221</v>
@@ -3040,7 +3046,7 @@
     </row>
     <row r="229" spans="1:2">
       <c r="A229" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B229">
         <v>0.02600780234070221</v>
@@ -3048,7 +3054,7 @@
     </row>
     <row r="230" spans="1:2">
       <c r="A230" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B230">
         <v>0.02600780234070221</v>
@@ -3056,7 +3062,7 @@
     </row>
     <row r="231" spans="1:2">
       <c r="A231" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B231">
         <v>0.02600780234070221</v>
@@ -3064,7 +3070,7 @@
     </row>
     <row r="232" spans="1:2">
       <c r="A232" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B232">
         <v>0.02600780234070221</v>
@@ -3072,7 +3078,7 @@
     </row>
     <row r="233" spans="1:2">
       <c r="A233" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B233">
         <v>0.02600780234070221</v>
@@ -3080,7 +3086,7 @@
     </row>
     <row r="234" spans="1:2">
       <c r="A234" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B234">
         <v>0.02600780234070221</v>
@@ -3088,7 +3094,7 @@
     </row>
     <row r="235" spans="1:2">
       <c r="A235" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B235">
         <v>0.02600780234070221</v>
@@ -3096,7 +3102,7 @@
     </row>
     <row r="236" spans="1:2">
       <c r="A236" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B236">
         <v>0.02600780234070221</v>
@@ -3104,7 +3110,7 @@
     </row>
     <row r="237" spans="1:2">
       <c r="A237" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B237">
         <v>0.02600780234070221</v>
@@ -3112,7 +3118,7 @@
     </row>
     <row r="238" spans="1:2">
       <c r="A238" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B238">
         <v>0.02600780234070221</v>
@@ -3120,7 +3126,7 @@
     </row>
     <row r="239" spans="1:2">
       <c r="A239" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B239">
         <v>0.02600780234070221</v>
@@ -3128,7 +3134,7 @@
     </row>
     <row r="240" spans="1:2">
       <c r="A240" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B240">
         <v>0.02600780234070221</v>
@@ -3136,7 +3142,7 @@
     </row>
     <row r="241" spans="1:2">
       <c r="A241" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B241">
         <v>0.02600780234070221</v>
@@ -3144,7 +3150,7 @@
     </row>
     <row r="242" spans="1:2">
       <c r="A242" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B242">
         <v>0.02600780234070221</v>
@@ -3152,7 +3158,7 @@
     </row>
     <row r="243" spans="1:2">
       <c r="A243" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B243">
         <v>0.02600780234070221</v>
@@ -3160,7 +3166,7 @@
     </row>
     <row r="244" spans="1:2">
       <c r="A244" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B244">
         <v>0.02600780234070221</v>
@@ -3168,7 +3174,7 @@
     </row>
     <row r="245" spans="1:2">
       <c r="A245" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B245">
         <v>0.02600780234070221</v>
@@ -3176,7 +3182,7 @@
     </row>
     <row r="246" spans="1:2">
       <c r="A246" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B246">
         <v>0.02600780234070221</v>
@@ -3184,7 +3190,7 @@
     </row>
     <row r="247" spans="1:2">
       <c r="A247" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B247">
         <v>0.02600780234070221</v>
@@ -3192,7 +3198,7 @@
     </row>
     <row r="248" spans="1:2">
       <c r="A248" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B248">
         <v>0.02600780234070221</v>
@@ -3200,7 +3206,7 @@
     </row>
     <row r="249" spans="1:2">
       <c r="A249" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B249">
         <v>0.02600780234070221</v>
@@ -3208,7 +3214,7 @@
     </row>
     <row r="250" spans="1:2">
       <c r="A250" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B250">
         <v>0.02600780234070221</v>
@@ -3216,7 +3222,7 @@
     </row>
     <row r="251" spans="1:2">
       <c r="A251" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B251">
         <v>0.02600780234070221</v>
@@ -3224,7 +3230,7 @@
     </row>
     <row r="252" spans="1:2">
       <c r="A252" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B252">
         <v>0.02600780234070221</v>
@@ -3232,7 +3238,7 @@
     </row>
     <row r="253" spans="1:2">
       <c r="A253" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B253">
         <v>0.02600780234070221</v>
@@ -3240,7 +3246,7 @@
     </row>
     <row r="254" spans="1:2">
       <c r="A254" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B254">
         <v>0.02600780234070221</v>
@@ -3248,7 +3254,7 @@
     </row>
     <row r="255" spans="1:2">
       <c r="A255" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B255">
         <v>0.02600780234070221</v>
@@ -3256,7 +3262,7 @@
     </row>
     <row r="256" spans="1:2">
       <c r="A256" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B256">
         <v>0.02600780234070221</v>
@@ -3264,7 +3270,7 @@
     </row>
     <row r="257" spans="1:2">
       <c r="A257" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B257">
         <v>0.02600780234070221</v>
@@ -3272,7 +3278,7 @@
     </row>
     <row r="258" spans="1:2">
       <c r="A258" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B258">
         <v>0.02600780234070221</v>
@@ -3280,7 +3286,7 @@
     </row>
     <row r="259" spans="1:2">
       <c r="A259" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B259">
         <v>0.02600780234070221</v>
@@ -3288,7 +3294,7 @@
     </row>
     <row r="260" spans="1:2">
       <c r="A260" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B260">
         <v>0.02600780234070221</v>
@@ -3296,7 +3302,7 @@
     </row>
     <row r="261" spans="1:2">
       <c r="A261" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B261">
         <v>0.02600780234070221</v>
@@ -3304,7 +3310,7 @@
     </row>
     <row r="262" spans="1:2">
       <c r="A262" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B262">
         <v>0.02600780234070221</v>
@@ -3312,7 +3318,7 @@
     </row>
     <row r="263" spans="1:2">
       <c r="A263" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B263">
         <v>0.02600780234070221</v>
@@ -3320,7 +3326,7 @@
     </row>
     <row r="264" spans="1:2">
       <c r="A264" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B264">
         <v>0.02600780234070221</v>
@@ -3328,7 +3334,7 @@
     </row>
     <row r="265" spans="1:2">
       <c r="A265" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B265">
         <v>0.02600780234070221</v>
@@ -3336,7 +3342,7 @@
     </row>
     <row r="266" spans="1:2">
       <c r="A266" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B266">
         <v>0.02600780234070221</v>
@@ -3344,7 +3350,7 @@
     </row>
     <row r="267" spans="1:2">
       <c r="A267" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B267">
         <v>0.02600780234070221</v>
@@ -3352,7 +3358,7 @@
     </row>
     <row r="268" spans="1:2">
       <c r="A268" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B268">
         <v>0.02600780234070221</v>
@@ -3360,7 +3366,7 @@
     </row>
     <row r="269" spans="1:2">
       <c r="A269" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B269">
         <v>0.02600780234070221</v>
@@ -3368,7 +3374,7 @@
     </row>
     <row r="270" spans="1:2">
       <c r="A270" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B270">
         <v>0.02600780234070221</v>
@@ -3376,7 +3382,7 @@
     </row>
     <row r="271" spans="1:2">
       <c r="A271" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B271">
         <v>0.02600780234070221</v>
@@ -3384,7 +3390,7 @@
     </row>
     <row r="272" spans="1:2">
       <c r="A272" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B272">
         <v>0.02600780234070221</v>
@@ -3392,7 +3398,7 @@
     </row>
     <row r="273" spans="1:2">
       <c r="A273" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B273">
         <v>0.02600780234070221</v>
@@ -3400,7 +3406,7 @@
     </row>
     <row r="274" spans="1:2">
       <c r="A274" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B274">
         <v>0.02600780234070221</v>
@@ -3408,7 +3414,7 @@
     </row>
     <row r="275" spans="1:2">
       <c r="A275" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B275">
         <v>0.02600780234070221</v>
@@ -3416,7 +3422,7 @@
     </row>
     <row r="276" spans="1:2">
       <c r="A276" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B276">
         <v>0.02600780234070221</v>
@@ -3424,7 +3430,7 @@
     </row>
     <row r="277" spans="1:2">
       <c r="A277" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B277">
         <v>0.02600780234070221</v>
@@ -3432,7 +3438,7 @@
     </row>
     <row r="278" spans="1:2">
       <c r="A278" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B278">
         <v>0.02600780234070221</v>
@@ -3440,7 +3446,7 @@
     </row>
     <row r="279" spans="1:2">
       <c r="A279" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B279">
         <v>0.02600780234070221</v>
@@ -3448,7 +3454,7 @@
     </row>
     <row r="280" spans="1:2">
       <c r="A280" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B280">
         <v>0.02600780234070221</v>

</xml_diff>